<commit_message>
Fixed header values and wrong data bug for pivot tables with date groupings.
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/PivotTables/PivotTableDateGrouping.xlsx
+++ b/EPPlusTest/Workbooks/PivotTables/PivotTableDateGrouping.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\EPPlus\EPPlusTest\Workbooks\PivotTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE7B26F-DD6B-4D3E-812D-DFA2E696DCFF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB6D7F8-7DF7-4C46-84A9-7A823DDC2112}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8880" activeTab="2" xr2:uid="{BFFA2122-528C-48FE-BDF2-B7EF1CD5D5DE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8880" activeTab="3" xr2:uid="{BFFA2122-528C-48FE-BDF2-B7EF1CD5D5DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="ColumnDataFields" sheetId="2" r:id="rId2"/>
     <sheet name="RowDataFields" sheetId="3" r:id="rId3"/>
+    <sheet name="PivotTables" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="11" r:id="rId4"/>
+    <pivotCache cacheId="2" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="90">
   <si>
     <t>Transaction</t>
   </si>
@@ -251,6 +252,60 @@
   </si>
   <si>
     <t>San Francisco Total</t>
+  </si>
+  <si>
+    <t>Feb Total</t>
+  </si>
+  <si>
+    <t>Mar Total</t>
+  </si>
+  <si>
+    <t>May Total</t>
+  </si>
+  <si>
+    <t>Oct Total</t>
+  </si>
+  <si>
+    <t>Nov Total</t>
+  </si>
+  <si>
+    <t>Dec Total</t>
+  </si>
+  <si>
+    <t>Feb Sum of Units Sold</t>
+  </si>
+  <si>
+    <t>Feb Sum of Total</t>
+  </si>
+  <si>
+    <t>Mar Sum of Units Sold</t>
+  </si>
+  <si>
+    <t>Mar Sum of Total</t>
+  </si>
+  <si>
+    <t>May Sum of Units Sold</t>
+  </si>
+  <si>
+    <t>May Sum of Total</t>
+  </si>
+  <si>
+    <t>Oct Sum of Units Sold</t>
+  </si>
+  <si>
+    <t>Oct Sum of Total</t>
+  </si>
+  <si>
+    <t>Nov Sum of Units Sold</t>
+  </si>
+  <si>
+    <t>Nov Sum of Total</t>
+  </si>
+  <si>
+    <t>Dec Sum of Units Sold</t>
+  </si>
+  <si>
+    <t>Dec Sum of Total</t>
   </si>
 </sst>
 </file>
@@ -326,7 +381,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -344,6 +399,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -537,7 +605,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A09B3987-AEB9-452C-AD74-CD92BAAEB057}" name="PivotTable1" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A09B3987-AEB9-452C-AD74-CD92BAAEB057}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:AE22" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField showAll="0"/>
@@ -787,7 +855,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AC9F801F-AC93-419C-9DFD-D809D2C6343C}" name="PivotTable1" cacheId="11" dataOnRows="1" dataPosition="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AC9F801F-AC93-419C-9DFD-D809D2C6343C}" name="PivotTable1" cacheId="2" dataOnRows="1" dataPosition="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:S78" firstHeaderRow="1" firstDataRow="5" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField axis="axisRow" showAll="0">
@@ -1178,6 +1246,860 @@
     </ext>
     <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
       <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{99026143-3B5D-49FF-BF3B-B658176C29BB}" name="PivotTable4" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A96:I123" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
+  <pivotFields count="9">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" numFmtId="14" showAll="0" sortType="ascending">
+      <items count="15">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="0"/>
+        <item x="13"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="8" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+    <pivotField axis="axisCol" showAll="0" sortType="descending" defaultSubtotal="0">
+      <items count="6">
+        <item sd="0" x="4"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="5"/>
+        <item sd="0" x="0"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" sortType="descending" defaultSubtotal="0">
+      <items count="5">
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="0"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="4">
+    <field x="1"/>
+    <field x="2"/>
+    <field x="8"/>
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="25">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="3">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="3">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="3">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="3">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="9"/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="3">
+      <x/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="10"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="3">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="11"/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="3">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="2">
+    <field x="-2"/>
+    <field x="7"/>
+  </colFields>
+  <colItems count="8">
+    <i>
+      <x/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="2"/>
+    </i>
+    <i r="1" i="1">
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{19A6443F-DE77-4F69-A519-113DE9575E09}" name="PivotTable3" cacheId="2" dataOnRows="1" dataPosition="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A35:H92" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
+  <pivotFields count="9">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" numFmtId="14" showAll="0" sortType="descending">
+      <items count="15">
+        <item x="13"/>
+        <item x="0"/>
+        <item x="12"/>
+        <item x="11"/>
+        <item x="10"/>
+        <item x="9"/>
+        <item x="8"/>
+        <item x="7"/>
+        <item x="6"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="8" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+    <pivotField axis="axisCol" showAll="0" sortType="descending" defaultSubtotal="0">
+      <items count="6">
+        <item x="4"/>
+        <item sd="0" x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item sd="0" x="5"/>
+        <item sd="0" x="0"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" sortType="descending" defaultSubtotal="0">
+      <items count="5">
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="0"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="4">
+    <field x="2"/>
+    <field x="8"/>
+    <field x="-2"/>
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="55">
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="3">
+      <x v="2"/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i r="3" i="1">
+      <x v="2"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i t="default" i="1">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="3">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i r="3" i="1">
+      <x/>
+    </i>
+    <i t="default">
+      <x v="3"/>
+    </i>
+    <i t="default" i="1">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="3">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i r="3" i="1">
+      <x/>
+    </i>
+    <i t="default">
+      <x v="4"/>
+    </i>
+    <i t="default" i="1">
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="3">
+      <x v="3"/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i r="3" i="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="3">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i r="3" i="1">
+      <x/>
+    </i>
+    <i t="default">
+      <x v="9"/>
+    </i>
+    <i t="default" i="1">
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="3">
+      <x v="1"/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i r="3" i="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="11"/>
+    </i>
+    <i t="default" i="1">
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="3">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i r="3" i="1">
+      <x/>
+    </i>
+    <i t="default">
+      <x v="12"/>
+    </i>
+    <i t="default" i="1">
+      <x v="12"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="2">
+    <field x="7"/>
+    <field x="1"/>
+  </colFields>
+  <colItems count="7">
+    <i>
+      <x/>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="3"/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{31630113-D71A-4EF1-B17C-E8CA73FEC0FD}" name="PivotTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="H1:V19" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
+  <pivotFields count="9">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" numFmtId="14" showAll="0" sortType="ascending">
+      <items count="15">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="0"/>
+        <item x="13"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="8" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="6">
+        <item x="4"/>
+        <item sd="0" x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item sd="0" x="5"/>
+        <item sd="0" x="0"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" sortType="ascending" defaultSubtotal="0">
+      <items count="5">
+        <item sd="0" x="0"/>
+        <item sd="0" x="4"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="3">
+    <field x="8"/>
+    <field x="7"/>
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="16">
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="2">
+    <field x="2"/>
+    <field x="1"/>
+  </colFields>
+  <colItems count="14">
+    <i>
+      <x v="1"/>
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="4"/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="9"/>
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+      <x v="2"/>
+    </i>
+    <i t="default">
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+      <x v="2"/>
+    </i>
+    <i t="default">
+      <x v="11"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Wholesale Price" fld="4" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1FC88330-B428-4CDE-9E21-FED589FFD62B}" name="PivotTable1" cacheId="2" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A1:E31" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="9">
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" numFmtId="14" showAll="0" sortType="descending" defaultSubtotal="0">
+      <items count="14">
+        <item x="13"/>
+        <item x="0"/>
+        <item x="12"/>
+        <item x="11"/>
+        <item x="10"/>
+        <item x="9"/>
+        <item x="8"/>
+        <item x="7"/>
+        <item x="6"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="8" showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0">
+      <items count="6">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0" defaultSubtotal="0">
+      <items count="5">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="3">
+    <field x="2"/>
+    <field x="3"/>
+    <field x="-2"/>
+  </rowFields>
+  <rowItems count="29">
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Wholesale Price" fld="4" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
     </ext>
   </extLst>
 </pivotTableDefinition>
@@ -2907,7 +3829,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DCB94E9-9699-4F62-A690-0ED99B841019}">
   <dimension ref="A1:S78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B43" workbookViewId="0">
+    <sheetView topLeftCell="B43" workbookViewId="0">
       <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
@@ -5195,4 +6117,2189 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E2E34A1-DAA8-417B-B43F-8512815E33C8}">
+  <dimension ref="A1:V123"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="E110" sqref="E110"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="25.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="P2" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q2" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="R2" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="S2" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="T2" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="U2" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="V2" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="H3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" t="s">
+        <v>9</v>
+      </c>
+      <c r="N3" t="s">
+        <v>11</v>
+      </c>
+      <c r="P3" t="s">
+        <v>11</v>
+      </c>
+      <c r="R3" t="s">
+        <v>6</v>
+      </c>
+      <c r="T3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="H4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8">
+        <v>99</v>
+      </c>
+      <c r="E5" s="8">
+        <v>99</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8">
+        <v>99</v>
+      </c>
+      <c r="E6" s="8">
+        <v>99</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8">
+        <v>415.75</v>
+      </c>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8">
+        <v>415.75</v>
+      </c>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="8"/>
+      <c r="U6" s="8"/>
+      <c r="V6" s="8">
+        <v>415.75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="H7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8"/>
+      <c r="S7" s="8"/>
+      <c r="T7" s="8"/>
+      <c r="U7" s="8"/>
+      <c r="V7" s="8"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="H8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8"/>
+      <c r="S8" s="8"/>
+      <c r="T8" s="8"/>
+      <c r="U8" s="8"/>
+      <c r="V8" s="8"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A9" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8">
+        <v>415.75</v>
+      </c>
+      <c r="E9" s="8">
+        <v>415.75</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8">
+        <v>415.75</v>
+      </c>
+      <c r="Q9" s="8">
+        <v>415.75</v>
+      </c>
+      <c r="R9" s="8"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="8"/>
+      <c r="U9" s="8"/>
+      <c r="V9" s="8">
+        <v>415.75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A10" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8">
+        <v>415.75</v>
+      </c>
+      <c r="E10" s="8">
+        <v>415.75</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="8"/>
+      <c r="T10" s="8">
+        <v>99</v>
+      </c>
+      <c r="U10" s="8">
+        <v>99</v>
+      </c>
+      <c r="V10" s="8">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="H11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="8"/>
+      <c r="T11" s="8"/>
+      <c r="U11" s="8"/>
+      <c r="V11" s="8"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="H12" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="8"/>
+      <c r="T12" s="8"/>
+      <c r="U12" s="8"/>
+      <c r="V12" s="8"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8">
+        <v>415.75</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8">
+        <v>415.75</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="8">
+        <v>415.75</v>
+      </c>
+      <c r="S13" s="8">
+        <v>415.75</v>
+      </c>
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
+      <c r="V13" s="8">
+        <v>415.75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A14" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8">
+        <v>831.5</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8">
+        <v>831.5</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
+      <c r="U14" s="8"/>
+      <c r="V14" s="8"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="H15" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8">
+        <v>199</v>
+      </c>
+      <c r="O15" s="8">
+        <v>199</v>
+      </c>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="8"/>
+      <c r="T15" s="8"/>
+      <c r="U15" s="8"/>
+      <c r="V15" s="8">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="H16" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="8"/>
+      <c r="T16" s="8"/>
+      <c r="U16" s="8"/>
+      <c r="V16" s="8"/>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A17" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="8">
+        <v>415.75</v>
+      </c>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8">
+        <v>415.75</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I17" s="8">
+        <v>415.75</v>
+      </c>
+      <c r="J17" s="8">
+        <v>415.75</v>
+      </c>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="8"/>
+      <c r="S17" s="8"/>
+      <c r="T17" s="8"/>
+      <c r="U17" s="8"/>
+      <c r="V17" s="8">
+        <v>415.75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A18" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="8">
+        <v>831.5</v>
+      </c>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8">
+        <v>831.5</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8">
+        <v>24.99</v>
+      </c>
+      <c r="L18" s="8">
+        <v>24.99</v>
+      </c>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
+      <c r="Q18" s="8"/>
+      <c r="R18" s="8"/>
+      <c r="S18" s="8"/>
+      <c r="T18" s="8"/>
+      <c r="U18" s="8"/>
+      <c r="V18" s="8">
+        <v>24.99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="H19" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" s="8">
+        <v>415.75</v>
+      </c>
+      <c r="J19" s="8">
+        <v>415.75</v>
+      </c>
+      <c r="K19" s="8">
+        <v>24.99</v>
+      </c>
+      <c r="L19" s="8">
+        <v>24.99</v>
+      </c>
+      <c r="M19" s="8">
+        <v>415.75</v>
+      </c>
+      <c r="N19" s="8">
+        <v>199</v>
+      </c>
+      <c r="O19" s="8">
+        <v>614.75</v>
+      </c>
+      <c r="P19" s="8">
+        <v>415.75</v>
+      </c>
+      <c r="Q19" s="8">
+        <v>415.75</v>
+      </c>
+      <c r="R19" s="8">
+        <v>415.75</v>
+      </c>
+      <c r="S19" s="8">
+        <v>415.75</v>
+      </c>
+      <c r="T19" s="8">
+        <v>99</v>
+      </c>
+      <c r="U19" s="8">
+        <v>99</v>
+      </c>
+      <c r="V19" s="8">
+        <v>1985.99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A20" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8">
+        <v>199</v>
+      </c>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A21" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8">
+        <v>1194</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A22" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A24" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="8">
+        <v>24.99</v>
+      </c>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8">
+        <v>24.99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A25" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="8">
+        <v>24.99</v>
+      </c>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8">
+        <v>24.99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A26" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A27" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A28" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8">
+        <v>415.75</v>
+      </c>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8">
+        <v>415.75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A29" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8">
+        <v>831.5</v>
+      </c>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8">
+        <v>831.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A30" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="8">
+        <v>440.74</v>
+      </c>
+      <c r="C30" s="8">
+        <v>1030.5</v>
+      </c>
+      <c r="D30" s="8">
+        <v>514.75</v>
+      </c>
+      <c r="E30" s="8">
+        <v>1985.99</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A31" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="8">
+        <v>856.49</v>
+      </c>
+      <c r="C31" s="8">
+        <v>2857</v>
+      </c>
+      <c r="D31" s="8">
+        <v>514.75</v>
+      </c>
+      <c r="E31" s="8">
+        <v>4228.24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B35" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>23</v>
+      </c>
+      <c r="D36" t="s">
+        <v>17</v>
+      </c>
+      <c r="F36" t="s">
+        <v>20</v>
+      </c>
+      <c r="H36" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" t="s">
+        <v>9</v>
+      </c>
+      <c r="G37" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8">
+        <v>1</v>
+      </c>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8">
+        <v>99</v>
+      </c>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B44" s="8"/>
+      <c r="C44" s="8">
+        <v>1</v>
+      </c>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B45" s="8"/>
+      <c r="C45" s="8">
+        <v>99</v>
+      </c>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B47" s="8"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="8"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B48" s="8"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="8"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A49" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B49" s="8"/>
+      <c r="C49" s="8">
+        <v>1</v>
+      </c>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A50" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B50" s="8"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="8"/>
+      <c r="H50" s="8"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B51" s="8"/>
+      <c r="C51" s="8">
+        <v>415.75</v>
+      </c>
+      <c r="D51" s="8"/>
+      <c r="E51" s="8"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="8"/>
+      <c r="H51" s="8">
+        <v>415.75</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A52" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B52" s="8"/>
+      <c r="C52" s="8">
+        <v>1</v>
+      </c>
+      <c r="D52" s="8"/>
+      <c r="E52" s="8"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A53" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B53" s="8"/>
+      <c r="C53" s="8">
+        <v>415.75</v>
+      </c>
+      <c r="D53" s="8"/>
+      <c r="E53" s="8"/>
+      <c r="F53" s="8"/>
+      <c r="G53" s="8"/>
+      <c r="H53" s="8">
+        <v>415.75</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A54" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B54" s="8"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="8"/>
+      <c r="E54" s="8"/>
+      <c r="F54" s="8"/>
+      <c r="G54" s="8"/>
+      <c r="H54" s="8"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A55" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B55" s="8"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="8"/>
+      <c r="E55" s="8"/>
+      <c r="F55" s="8"/>
+      <c r="G55" s="8"/>
+      <c r="H55" s="8"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A56" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B56" s="8"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="8"/>
+      <c r="E56" s="8"/>
+      <c r="F56" s="8"/>
+      <c r="G56" s="8"/>
+      <c r="H56" s="8"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A57" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B57" s="8">
+        <v>2</v>
+      </c>
+      <c r="C57" s="8"/>
+      <c r="D57" s="8"/>
+      <c r="E57" s="8"/>
+      <c r="F57" s="8"/>
+      <c r="G57" s="8"/>
+      <c r="H57" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A58" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B58" s="8"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
+      <c r="E58" s="8"/>
+      <c r="F58" s="8"/>
+      <c r="G58" s="8"/>
+      <c r="H58" s="8"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A59" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B59" s="8">
+        <v>831.5</v>
+      </c>
+      <c r="C59" s="8"/>
+      <c r="D59" s="8"/>
+      <c r="E59" s="8"/>
+      <c r="F59" s="8"/>
+      <c r="G59" s="8"/>
+      <c r="H59" s="8">
+        <v>831.5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A60" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B60" s="8">
+        <v>2</v>
+      </c>
+      <c r="C60" s="8"/>
+      <c r="D60" s="8"/>
+      <c r="E60" s="8"/>
+      <c r="F60" s="8"/>
+      <c r="G60" s="8"/>
+      <c r="H60" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A61" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B61" s="8">
+        <v>831.5</v>
+      </c>
+      <c r="C61" s="8"/>
+      <c r="D61" s="8"/>
+      <c r="E61" s="8"/>
+      <c r="F61" s="8"/>
+      <c r="G61" s="8"/>
+      <c r="H61" s="8">
+        <v>831.5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A62" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B62" s="8"/>
+      <c r="C62" s="8"/>
+      <c r="D62" s="8"/>
+      <c r="E62" s="8"/>
+      <c r="F62" s="8"/>
+      <c r="G62" s="8"/>
+      <c r="H62" s="8"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A63" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B63" s="8"/>
+      <c r="C63" s="8"/>
+      <c r="D63" s="8"/>
+      <c r="E63" s="8"/>
+      <c r="F63" s="8"/>
+      <c r="G63" s="8"/>
+      <c r="H63" s="8"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A64" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B64" s="8"/>
+      <c r="C64" s="8"/>
+      <c r="D64" s="8"/>
+      <c r="E64" s="8"/>
+      <c r="F64" s="8"/>
+      <c r="G64" s="8"/>
+      <c r="H64" s="8"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A65" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B65" s="8"/>
+      <c r="C65" s="8"/>
+      <c r="D65" s="8"/>
+      <c r="E65" s="8">
+        <v>6</v>
+      </c>
+      <c r="F65" s="8"/>
+      <c r="G65" s="8"/>
+      <c r="H65" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A66" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B66" s="8"/>
+      <c r="C66" s="8"/>
+      <c r="D66" s="8"/>
+      <c r="E66" s="8"/>
+      <c r="F66" s="8"/>
+      <c r="G66" s="8"/>
+      <c r="H66" s="8"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A67" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B67" s="8"/>
+      <c r="C67" s="8"/>
+      <c r="D67" s="8"/>
+      <c r="E67" s="8">
+        <v>1194</v>
+      </c>
+      <c r="F67" s="8"/>
+      <c r="G67" s="8"/>
+      <c r="H67" s="8">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A68" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B68" s="8"/>
+      <c r="C68" s="8"/>
+      <c r="D68" s="8"/>
+      <c r="E68" s="8"/>
+      <c r="F68" s="8"/>
+      <c r="G68" s="8"/>
+      <c r="H68" s="8"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A69" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B69" s="8"/>
+      <c r="C69" s="8"/>
+      <c r="D69" s="8"/>
+      <c r="E69" s="8"/>
+      <c r="F69" s="8"/>
+      <c r="G69" s="8"/>
+      <c r="H69" s="8"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A70" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B70" s="8"/>
+      <c r="C70" s="8"/>
+      <c r="D70" s="8">
+        <v>2</v>
+      </c>
+      <c r="E70" s="8"/>
+      <c r="F70" s="8"/>
+      <c r="G70" s="8"/>
+      <c r="H70" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A71" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B71" s="8"/>
+      <c r="C71" s="8"/>
+      <c r="D71" s="8"/>
+      <c r="E71" s="8"/>
+      <c r="F71" s="8"/>
+      <c r="G71" s="8"/>
+      <c r="H71" s="8"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A72" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B72" s="8"/>
+      <c r="C72" s="8"/>
+      <c r="D72" s="8">
+        <v>831.5</v>
+      </c>
+      <c r="E72" s="8"/>
+      <c r="F72" s="8"/>
+      <c r="G72" s="8"/>
+      <c r="H72" s="8">
+        <v>831.5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A73" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B73" s="8"/>
+      <c r="C73" s="8"/>
+      <c r="D73" s="8">
+        <v>2</v>
+      </c>
+      <c r="E73" s="8">
+        <v>6</v>
+      </c>
+      <c r="F73" s="8"/>
+      <c r="G73" s="8"/>
+      <c r="H73" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A74" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B74" s="8"/>
+      <c r="C74" s="8"/>
+      <c r="D74" s="8">
+        <v>831.5</v>
+      </c>
+      <c r="E74" s="8">
+        <v>1194</v>
+      </c>
+      <c r="F74" s="8"/>
+      <c r="G74" s="8"/>
+      <c r="H74" s="8">
+        <v>2025.5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A75" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B75" s="8"/>
+      <c r="C75" s="8"/>
+      <c r="D75" s="8"/>
+      <c r="E75" s="8"/>
+      <c r="F75" s="8"/>
+      <c r="G75" s="8"/>
+      <c r="H75" s="8"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A76" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B76" s="8"/>
+      <c r="C76" s="8"/>
+      <c r="D76" s="8"/>
+      <c r="E76" s="8"/>
+      <c r="F76" s="8"/>
+      <c r="G76" s="8"/>
+      <c r="H76" s="8"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A77" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B77" s="8"/>
+      <c r="C77" s="8"/>
+      <c r="D77" s="8"/>
+      <c r="E77" s="8"/>
+      <c r="F77" s="8"/>
+      <c r="G77" s="8"/>
+      <c r="H77" s="8"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A78" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B78" s="8"/>
+      <c r="C78" s="8"/>
+      <c r="D78" s="8"/>
+      <c r="E78" s="8"/>
+      <c r="F78" s="8">
+        <v>1</v>
+      </c>
+      <c r="G78" s="8"/>
+      <c r="H78" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A79" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B79" s="8"/>
+      <c r="C79" s="8"/>
+      <c r="D79" s="8"/>
+      <c r="E79" s="8"/>
+      <c r="F79" s="8"/>
+      <c r="G79" s="8"/>
+      <c r="H79" s="8"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A80" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B80" s="8"/>
+      <c r="C80" s="8"/>
+      <c r="D80" s="8"/>
+      <c r="E80" s="8"/>
+      <c r="F80" s="8">
+        <v>24.99</v>
+      </c>
+      <c r="G80" s="8"/>
+      <c r="H80" s="8">
+        <v>24.99</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A81" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B81" s="8"/>
+      <c r="C81" s="8"/>
+      <c r="D81" s="8"/>
+      <c r="E81" s="8"/>
+      <c r="F81" s="8">
+        <v>1</v>
+      </c>
+      <c r="G81" s="8"/>
+      <c r="H81" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A82" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B82" s="8"/>
+      <c r="C82" s="8"/>
+      <c r="D82" s="8"/>
+      <c r="E82" s="8"/>
+      <c r="F82" s="8">
+        <v>24.99</v>
+      </c>
+      <c r="G82" s="8"/>
+      <c r="H82" s="8">
+        <v>24.99</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A83" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B83" s="8"/>
+      <c r="C83" s="8"/>
+      <c r="D83" s="8"/>
+      <c r="E83" s="8"/>
+      <c r="F83" s="8"/>
+      <c r="G83" s="8"/>
+      <c r="H83" s="8"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A84" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B84" s="8"/>
+      <c r="C84" s="8"/>
+      <c r="D84" s="8"/>
+      <c r="E84" s="8"/>
+      <c r="F84" s="8"/>
+      <c r="G84" s="8"/>
+      <c r="H84" s="8"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A85" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B85" s="8"/>
+      <c r="C85" s="8"/>
+      <c r="D85" s="8"/>
+      <c r="E85" s="8"/>
+      <c r="F85" s="8"/>
+      <c r="G85" s="8"/>
+      <c r="H85" s="8"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A86" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B86" s="8"/>
+      <c r="C86" s="8"/>
+      <c r="D86" s="8"/>
+      <c r="E86" s="8"/>
+      <c r="F86" s="8"/>
+      <c r="G86" s="8">
+        <v>2</v>
+      </c>
+      <c r="H86" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A87" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B87" s="8"/>
+      <c r="C87" s="8"/>
+      <c r="D87" s="8"/>
+      <c r="E87" s="8"/>
+      <c r="F87" s="8"/>
+      <c r="G87" s="8"/>
+      <c r="H87" s="8"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A88" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B88" s="8"/>
+      <c r="C88" s="8"/>
+      <c r="D88" s="8"/>
+      <c r="E88" s="8"/>
+      <c r="F88" s="8"/>
+      <c r="G88" s="8">
+        <v>831.5</v>
+      </c>
+      <c r="H88" s="8">
+        <v>831.5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A89" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B89" s="8"/>
+      <c r="C89" s="8"/>
+      <c r="D89" s="8"/>
+      <c r="E89" s="8"/>
+      <c r="F89" s="8"/>
+      <c r="G89" s="8">
+        <v>2</v>
+      </c>
+      <c r="H89" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A90" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B90" s="8"/>
+      <c r="C90" s="8"/>
+      <c r="D90" s="8"/>
+      <c r="E90" s="8"/>
+      <c r="F90" s="8"/>
+      <c r="G90" s="8">
+        <v>831.5</v>
+      </c>
+      <c r="H90" s="8">
+        <v>831.5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A91" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B91" s="8">
+        <v>2</v>
+      </c>
+      <c r="C91" s="8">
+        <v>2</v>
+      </c>
+      <c r="D91" s="8">
+        <v>2</v>
+      </c>
+      <c r="E91" s="8">
+        <v>6</v>
+      </c>
+      <c r="F91" s="8">
+        <v>1</v>
+      </c>
+      <c r="G91" s="8">
+        <v>2</v>
+      </c>
+      <c r="H91" s="8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A92" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B92" s="8">
+        <v>831.5</v>
+      </c>
+      <c r="C92" s="8">
+        <v>514.75</v>
+      </c>
+      <c r="D92" s="8">
+        <v>831.5</v>
+      </c>
+      <c r="E92" s="8">
+        <v>1194</v>
+      </c>
+      <c r="F92" s="8">
+        <v>24.99</v>
+      </c>
+      <c r="G92" s="8">
+        <v>831.5</v>
+      </c>
+      <c r="H92" s="8">
+        <v>4228.24</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B96" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B97" t="s">
+        <v>29</v>
+      </c>
+      <c r="E97" t="s">
+        <v>30</v>
+      </c>
+      <c r="H97" t="s">
+        <v>33</v>
+      </c>
+      <c r="I97" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A98" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B98" t="s">
+        <v>23</v>
+      </c>
+      <c r="C98" t="s">
+        <v>17</v>
+      </c>
+      <c r="D98" t="s">
+        <v>20</v>
+      </c>
+      <c r="E98" t="s">
+        <v>23</v>
+      </c>
+      <c r="F98" t="s">
+        <v>17</v>
+      </c>
+      <c r="G98" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A99" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B99" s="8"/>
+      <c r="C99" s="8">
+        <v>2</v>
+      </c>
+      <c r="D99" s="8">
+        <v>1</v>
+      </c>
+      <c r="E99" s="8"/>
+      <c r="F99" s="8">
+        <v>831.5</v>
+      </c>
+      <c r="G99" s="8">
+        <v>24.99</v>
+      </c>
+      <c r="H99" s="8">
+        <v>3</v>
+      </c>
+      <c r="I99" s="8">
+        <v>856.49</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A100" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B100" s="8"/>
+      <c r="C100" s="8"/>
+      <c r="D100" s="8">
+        <v>1</v>
+      </c>
+      <c r="E100" s="8"/>
+      <c r="F100" s="8"/>
+      <c r="G100" s="8">
+        <v>24.99</v>
+      </c>
+      <c r="H100" s="8">
+        <v>1</v>
+      </c>
+      <c r="I100" s="8">
+        <v>24.99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A101" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B101" s="8"/>
+      <c r="C101" s="8"/>
+      <c r="D101" s="8"/>
+      <c r="E101" s="8"/>
+      <c r="F101" s="8"/>
+      <c r="G101" s="8"/>
+      <c r="H101" s="8"/>
+      <c r="I101" s="8"/>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A102" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B102" s="8"/>
+      <c r="C102" s="8"/>
+      <c r="D102" s="8">
+        <v>1</v>
+      </c>
+      <c r="E102" s="8"/>
+      <c r="F102" s="8"/>
+      <c r="G102" s="8">
+        <v>24.99</v>
+      </c>
+      <c r="H102" s="8">
+        <v>1</v>
+      </c>
+      <c r="I102" s="8">
+        <v>24.99</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A103" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B103" s="8"/>
+      <c r="C103" s="8">
+        <v>2</v>
+      </c>
+      <c r="D103" s="8"/>
+      <c r="E103" s="8"/>
+      <c r="F103" s="8">
+        <v>831.5</v>
+      </c>
+      <c r="G103" s="8"/>
+      <c r="H103" s="8">
+        <v>2</v>
+      </c>
+      <c r="I103" s="8">
+        <v>831.5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A104" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B104" s="8"/>
+      <c r="C104" s="8"/>
+      <c r="D104" s="8"/>
+      <c r="E104" s="8"/>
+      <c r="F104" s="8"/>
+      <c r="G104" s="8"/>
+      <c r="H104" s="8"/>
+      <c r="I104" s="8"/>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A105" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B105" s="8"/>
+      <c r="C105" s="8">
+        <v>2</v>
+      </c>
+      <c r="D105" s="8"/>
+      <c r="E105" s="8"/>
+      <c r="F105" s="8">
+        <v>831.5</v>
+      </c>
+      <c r="G105" s="8"/>
+      <c r="H105" s="8">
+        <v>2</v>
+      </c>
+      <c r="I105" s="8">
+        <v>831.5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A106" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B106" s="8">
+        <v>2</v>
+      </c>
+      <c r="C106" s="8">
+        <v>6</v>
+      </c>
+      <c r="D106" s="8">
+        <v>2</v>
+      </c>
+      <c r="E106" s="8">
+        <v>831.5</v>
+      </c>
+      <c r="F106" s="8">
+        <v>1194</v>
+      </c>
+      <c r="G106" s="8">
+        <v>831.5</v>
+      </c>
+      <c r="H106" s="8">
+        <v>10</v>
+      </c>
+      <c r="I106" s="8">
+        <v>2857</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A107" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B107" s="8"/>
+      <c r="C107" s="8"/>
+      <c r="D107" s="8">
+        <v>2</v>
+      </c>
+      <c r="E107" s="8"/>
+      <c r="F107" s="8"/>
+      <c r="G107" s="8">
+        <v>831.5</v>
+      </c>
+      <c r="H107" s="8">
+        <v>2</v>
+      </c>
+      <c r="I107" s="8">
+        <v>831.5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A108" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B108" s="8"/>
+      <c r="C108" s="8"/>
+      <c r="D108" s="8"/>
+      <c r="E108" s="8"/>
+      <c r="F108" s="8"/>
+      <c r="G108" s="8"/>
+      <c r="H108" s="8"/>
+      <c r="I108" s="8"/>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A109" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B109" s="8"/>
+      <c r="C109" s="8"/>
+      <c r="D109" s="8">
+        <v>2</v>
+      </c>
+      <c r="E109" s="8"/>
+      <c r="F109" s="8"/>
+      <c r="G109" s="8">
+        <v>831.5</v>
+      </c>
+      <c r="H109" s="8">
+        <v>2</v>
+      </c>
+      <c r="I109" s="8">
+        <v>831.5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A110" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B110" s="8"/>
+      <c r="C110" s="8">
+        <v>6</v>
+      </c>
+      <c r="D110" s="8"/>
+      <c r="E110" s="8"/>
+      <c r="F110" s="8">
+        <v>1194</v>
+      </c>
+      <c r="G110" s="8"/>
+      <c r="H110" s="8">
+        <v>6</v>
+      </c>
+      <c r="I110" s="8">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A111" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B111" s="8"/>
+      <c r="C111" s="8"/>
+      <c r="D111" s="8"/>
+      <c r="E111" s="8"/>
+      <c r="F111" s="8"/>
+      <c r="G111" s="8"/>
+      <c r="H111" s="8"/>
+      <c r="I111" s="8"/>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A112" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B112" s="8"/>
+      <c r="C112" s="8">
+        <v>6</v>
+      </c>
+      <c r="D112" s="8"/>
+      <c r="E112" s="8"/>
+      <c r="F112" s="8">
+        <v>1194</v>
+      </c>
+      <c r="G112" s="8"/>
+      <c r="H112" s="8">
+        <v>6</v>
+      </c>
+      <c r="I112" s="8">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A113" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B113" s="8">
+        <v>2</v>
+      </c>
+      <c r="C113" s="8"/>
+      <c r="D113" s="8"/>
+      <c r="E113" s="8">
+        <v>831.5</v>
+      </c>
+      <c r="F113" s="8"/>
+      <c r="G113" s="8"/>
+      <c r="H113" s="8">
+        <v>2</v>
+      </c>
+      <c r="I113" s="8">
+        <v>831.5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A114" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B114" s="8"/>
+      <c r="C114" s="8"/>
+      <c r="D114" s="8"/>
+      <c r="E114" s="8"/>
+      <c r="F114" s="8"/>
+      <c r="G114" s="8"/>
+      <c r="H114" s="8"/>
+      <c r="I114" s="8"/>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A115" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B115" s="8">
+        <v>2</v>
+      </c>
+      <c r="C115" s="8"/>
+      <c r="D115" s="8"/>
+      <c r="E115" s="8">
+        <v>831.5</v>
+      </c>
+      <c r="F115" s="8"/>
+      <c r="G115" s="8"/>
+      <c r="H115" s="8">
+        <v>2</v>
+      </c>
+      <c r="I115" s="8">
+        <v>831.5</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A116" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B116" s="8">
+        <v>2</v>
+      </c>
+      <c r="C116" s="8"/>
+      <c r="D116" s="8"/>
+      <c r="E116" s="8">
+        <v>514.75</v>
+      </c>
+      <c r="F116" s="8"/>
+      <c r="G116" s="8"/>
+      <c r="H116" s="8">
+        <v>2</v>
+      </c>
+      <c r="I116" s="8">
+        <v>514.75</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A117" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B117" s="8">
+        <v>1</v>
+      </c>
+      <c r="C117" s="8"/>
+      <c r="D117" s="8"/>
+      <c r="E117" s="8">
+        <v>415.75</v>
+      </c>
+      <c r="F117" s="8"/>
+      <c r="G117" s="8"/>
+      <c r="H117" s="8">
+        <v>1</v>
+      </c>
+      <c r="I117" s="8">
+        <v>415.75</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A118" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B118" s="8"/>
+      <c r="C118" s="8"/>
+      <c r="D118" s="8"/>
+      <c r="E118" s="8"/>
+      <c r="F118" s="8"/>
+      <c r="G118" s="8"/>
+      <c r="H118" s="8"/>
+      <c r="I118" s="8"/>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A119" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B119" s="8">
+        <v>1</v>
+      </c>
+      <c r="C119" s="8"/>
+      <c r="D119" s="8"/>
+      <c r="E119" s="8">
+        <v>415.75</v>
+      </c>
+      <c r="F119" s="8"/>
+      <c r="G119" s="8"/>
+      <c r="H119" s="8">
+        <v>1</v>
+      </c>
+      <c r="I119" s="8">
+        <v>415.75</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A120" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B120" s="8">
+        <v>1</v>
+      </c>
+      <c r="C120" s="8"/>
+      <c r="D120" s="8"/>
+      <c r="E120" s="8">
+        <v>99</v>
+      </c>
+      <c r="F120" s="8"/>
+      <c r="G120" s="8"/>
+      <c r="H120" s="8">
+        <v>1</v>
+      </c>
+      <c r="I120" s="8">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A121" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B121" s="8"/>
+      <c r="C121" s="8"/>
+      <c r="D121" s="8"/>
+      <c r="E121" s="8"/>
+      <c r="F121" s="8"/>
+      <c r="G121" s="8"/>
+      <c r="H121" s="8"/>
+      <c r="I121" s="8"/>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A122" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B122" s="8">
+        <v>1</v>
+      </c>
+      <c r="C122" s="8"/>
+      <c r="D122" s="8"/>
+      <c r="E122" s="8">
+        <v>99</v>
+      </c>
+      <c r="F122" s="8"/>
+      <c r="G122" s="8"/>
+      <c r="H122" s="8">
+        <v>1</v>
+      </c>
+      <c r="I122" s="8">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A123" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B123" s="8">
+        <v>4</v>
+      </c>
+      <c r="C123" s="8">
+        <v>8</v>
+      </c>
+      <c r="D123" s="8">
+        <v>3</v>
+      </c>
+      <c r="E123" s="8">
+        <v>1346.25</v>
+      </c>
+      <c r="F123" s="8">
+        <v>2025.5</v>
+      </c>
+      <c r="G123" s="8">
+        <v>856.49</v>
+      </c>
+      <c r="H123" s="8">
+        <v>15</v>
+      </c>
+      <c r="I123" s="8">
+        <v>4228.24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>